<commit_message>
update .gitignore for .DS_Store
</commit_message>
<xml_diff>
--- a/doc/resultaten.xlsx
+++ b/doc/resultaten.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c5535c1db43cb11/Documents/UvA/Minprog/problems/theorie/RoosterRulers/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E1241F3-0B12-4ED3-A11E-71487FEED3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{3E1241F3-0B12-4ED3-A11E-71487FEED3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DD9F497-54E7-48F4-8337-C43EC35C0AF2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{576B34F7-214E-4A40-AA32-36EEA87275C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{576B34F7-214E-4A40-AA32-36EEA87275C8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hillclimber" sheetId="1" r:id="rId1"/>
+    <sheet name="Simulated annealing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>runtime</t>
   </si>
@@ -131,6 +132,21 @@
   </si>
   <si>
     <t>pickled_schedule_hillclimber_21_06_2022_14_23.pickle</t>
+  </si>
+  <si>
+    <t>simulated annealing lessons -&gt; temperature</t>
+  </si>
+  <si>
+    <t>simulated annealing lessons -&gt; repeats</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -490,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A674BF-2D24-4795-A0A9-18E8DB2C376C}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,8 +786,173 @@
         <v>30</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>500</v>
+      </c>
+      <c r="B11">
+        <v>800</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>800</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10F971C-EB65-4D52-8185-5CC39B2A6CA6}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>10000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>30000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>30000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>30000</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <v>300</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>